<commit_message>
feat(problemas-promodel): agregar datos para problema 11, 200 números
</commit_message>
<xml_diff>
--- a/problemas-seccion-1.6-promodel/spreadsheets/problem-11-spreadsheet.xlsx
+++ b/problemas-seccion-1.6-promodel/spreadsheets/problem-11-spreadsheet.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\tusch\mi415-preview\problemas-seccion-1.6-promodel\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC9F49A-E11D-4485-8934-6B110DC33717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EA519F-436A-4E4D-B5F4-48308C5C59AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{02BBDC00-C366-48A1-939B-7E66C0C7C583}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="1" activeTab="3" xr2:uid="{02BBDC00-C366-48A1-939B-7E66C0C7C583}"/>
   </bookViews>
   <sheets>
-    <sheet name="random-numbers-original" sheetId="1" r:id="rId1"/>
-    <sheet name="random-numbers-transformed" sheetId="2" r:id="rId2"/>
+    <sheet name="random-100-numbers-original" sheetId="1" r:id="rId1"/>
+    <sheet name="random-100-numbers-transformed" sheetId="2" r:id="rId2"/>
+    <sheet name="random-200-numbers-original" sheetId="3" r:id="rId3"/>
+    <sheet name="random-200-numbers-transformed" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -70,7 +72,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,7 +389,523 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3331D668-FEB8-4704-B8F5-FFFA48AC7974}">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0.47746674003147993</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0.4121860784418141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.29974572121892118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.56101433182835725</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.55340087545256544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.12173770371858883</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.23591839838028472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.25599624348363503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.21561805827047964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.77769711241114758</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>7.2201153758782555E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.35658824492248831</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.95707544522696097</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.15828870625869995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.93051757374708854</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.706012802357324</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.83580276587677027</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.33859229070276686</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.68482638464682033</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.59080562509132128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0.13061481463620772</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0.87862231268230684</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0.21030505098181917</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0.67125903139592147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0.80156909309987046</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0.28700444505885914</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>0.38031874366396778</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>0.3847025518656243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>0.72507441316045818</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>5.6846604292582148E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>0.74878769300904491</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>0.51577663502655535</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>0.70248468191158819</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>0.29804641989590397</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>0.80217826847966023</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>0.27360321483111261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>0.50205284478587009</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>0.64132877785020181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>0.45680347095622686</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>0.91980467886125239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>0.50056702642546314</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>0.47251171288553762</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>0.17183954107414368</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>0.12683478718722929</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>0.51663475381000712</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>0.87764976845918663</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>0.59281364130360203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>0.27765774707308455</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>0.55160359454552976</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>0.88444846525767329</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>0.68051185098410272</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>0.19435677158345177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>0.10137949954451664</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>0.70615536769550957</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>0.99159974975147636</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>0.67128362921582718</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>0.53859857468323213</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>0.17651591222443952</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>0.8419481984198337</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>2.3042630015838617E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>0.67938690941989555</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>0.71380958119073168</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>0.97253350388913717</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>0.42778886433236385</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>0.64072052732553819</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>0.71461827184781024</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>0.47871123374656832</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>0.84364800010689878</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>0.82170177756537965</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>0.18617563148524674</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>0.78037758617160635</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>0.83981387431186916</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>0.39692228099127624</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>0.10089576241638509</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>0.85954648388976018</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>5.9656712172234005E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>0.62816946494723491</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>0.19892154522212557</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>0.59267244806953845</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>0.51817035212066187</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>0.39255297222211183</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>0.54693143168641889</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>0.76123607523522163</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>0.45069833677117455</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>0.57469175675568895</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>0.56864190888627564</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>0.92376716786498192</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>0.80922055662557812</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>0.74822701327122476</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>0.97772429420837514</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>0.38804907369484332</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>0.81690355843927831</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>0.23781090068026633</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>0.72144630776841023</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>1.1142469896511242E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>7.8631740363009461E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>9.5274252332576248E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>4.1135510269063702E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>6.1715924717818504E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>0.21797932485098637</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BD8CAE-D53D-4F1C-B0AF-70A90225B578}">
+  <dimension ref="A1:A100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A100"/>
     </sheetView>
   </sheetViews>
@@ -398,502 +916,602 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>0.47746674003147993</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A1)</f>
+        <v>1.9471999251808469</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.4121860784418141</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A2)</f>
+        <v>1.5940345233077402</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.29974572121892118</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A3)</f>
+        <v>1.0689352634953835</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.56101433182835725</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A4)</f>
+        <v>2.4698655389211561</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>0.55340087545256544</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A5)</f>
+        <v>2.4182816995170215</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.12173770371858883</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A6)</f>
+        <v>0.38942996113342676</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0.23591839838028472</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A7)</f>
+        <v>0.80724206134937759</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.25599624348363503</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A8)</f>
+        <v>0.88712758524196822</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0.21561805827047964</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A9)</f>
+        <v>0.72857762006225502</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>0.77769711241114758</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A10)</f>
+        <v>4.5111434054786272</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>7.2201153758782555E-2</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A11)</f>
+        <v>0.22482099062346594</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>0.35658824492248831</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A12)</f>
+        <v>1.3229111822885704</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0.95707544522696097</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A13)</f>
+        <v>9.4449337333764554</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>0.15828870625869995</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A14)</f>
+        <v>0.51695461523857833</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>0.93051757374708854</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A15)</f>
+        <v>8.0000442541683778</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>0.706012802357324</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A16)</f>
+        <v>3.6726571740739802</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>0.83580276587677027</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A17)</f>
+        <v>5.4200607799973746</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>0.33859229070276686</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A18)</f>
+        <v>1.2401544674217029</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>0.68482638464682033</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A19)</f>
+        <v>3.4638948964138319</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0.59080562509132128</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A20)</f>
+        <v>2.6806949746698949</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>0.13061481463620772</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A21)</f>
+        <v>0.41990700192564312</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>0.87862231268230684</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A22)</f>
+        <v>6.3265446359887108</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>0.21030505098181917</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A23)</f>
+        <v>0.70832564572745715</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>0.67125903139592147</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A24)</f>
+        <v>3.3374555033828415</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>0.80156909309987046</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A25)</f>
+        <v>4.8519429465519135</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>0.28700444505885914</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A26)</f>
+        <v>1.0148402786742743</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>0.38031874366396778</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A27)</f>
+        <v>1.4356501074687413</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>0.3847025518656243</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A28)</f>
+        <v>1.4569484177885792</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>0.72507441316045818</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A29)</f>
+        <v>3.8737644337298951</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>5.6846604292582148E-2</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A30)</f>
+        <v>0.17557902542196074</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>0.74878769300904491</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A31)</f>
+        <v>4.1443705583694399</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>0.51577663502655535</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A32)</f>
+        <v>2.175626942531645</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>0.70248468191158819</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A33)</f>
+        <v>3.6368686978475164</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>0.29804641989590397</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A34)</f>
+        <v>1.0616640070516028</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>0.80217826847966023</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A35)</f>
+        <v>4.8611669990977422</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>0.27360321483111261</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A36)</f>
+        <v>0.95897663222541341</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>0.50205284478587009</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A37)</f>
+        <v>2.0917839648474823</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>0.64132877785020181</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A38)</f>
+        <v>3.0760473775440862</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>0.45680347095622686</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A39)</f>
+        <v>1.8308522777673499</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>0.91980467886125239</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A40)</f>
+        <v>7.5698703171821169</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>0.50056702642546314</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A41)</f>
+        <v>2.0828456308061374</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>0.47251171288553762</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A42)</f>
+        <v>1.9188858552023573</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>0.17183954107414368</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A43)</f>
+        <v>0.565645057195998</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>0.12683478718722929</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A44)</f>
+        <v>0.40689148151794485</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>0.51663475381000712</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A45)</f>
+        <v>2.1809481234459041</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>0.87764976845918663</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A46)</f>
+        <v>6.302602789946631</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>0.59281364130360203</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A47)</f>
+        <v>2.6954529436841868</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>0.27765774707308455</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A48)</f>
+        <v>0.97576865365010579</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>0.55160359454552976</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A49)</f>
+        <v>2.4062328125937267</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>0.88444846525767329</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A50)</f>
+        <v>6.4741159808622335</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>0.68051185098410272</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A51)</f>
+        <v>3.4231052944034852</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>0.19435677158345177</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A52)</f>
+        <v>0.64834283734814957</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>0.10137949954451664</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A53)</f>
+        <v>0.3206834065030425</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>0.70615536769550957</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A54)</f>
+        <v>3.67411233863348</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>0.99159974975147636</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A55)</f>
+        <v>14.338481346257151</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>0.67128362921582718</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A56)</f>
+        <v>3.337679984745602</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>0.53859857468323213</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A57)</f>
+        <v>2.3204605324025724</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>0.17651591222443952</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A58)</f>
+        <v>0.58263315668412718</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>0.8419481984198337</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A59)</f>
+        <v>5.5344973247597249</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>2.3042630015838617E-2</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A60)</f>
+        <v>6.9936784439094526E-2</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>0.67938690941989555</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A61)</f>
+        <v>3.4125606244095321</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>0.71380958119073168</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A62)</f>
+        <v>3.7532936690291629</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>0.97253350388913717</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A63)</f>
+        <v>10.784365020930196</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>0.42778886433236385</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A64)</f>
+        <v>1.6747417122290291</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>0.64072052732553819</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A65)</f>
+        <v>3.0709641537970516</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>0.71461827184781024</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A66)</f>
+        <v>3.7617827936409185</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>0.47871123374656832</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A67)</f>
+        <v>1.9543534107760285</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>0.84364800010689878</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A68)</f>
+        <v>5.5669362120917025</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>0.82170177756537965</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A69)</f>
+        <v>5.1728931710476038</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>0.18617563148524674</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A70)</f>
+        <v>0.6180320992658328</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>0.78037758617160635</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A71)</f>
+        <v>4.547536523824169</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>0.83981387431186916</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A72)</f>
+        <v>5.4942565628695617</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>0.39692228099127624</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A73)</f>
+        <v>1.517127609945653</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>0.10089576241638509</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A74)</f>
+        <v>0.31906890858941545</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>0.85954648388976018</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A75)</f>
+        <v>5.8886360734214271</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>5.9656712172234005E-2</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A76)</f>
+        <v>0.18453081171161098</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>0.62816946494723491</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A77)</f>
+        <v>2.9679512383118034</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>0.19892154522212557</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A78)</f>
+        <v>0.66538917201115411</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>0.59267244806953845</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A79)</f>
+        <v>2.6944128639485134</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>0.51817035212066187</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A80)</f>
+        <v>2.190493965114094</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>0.39255297222211183</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A81)</f>
+        <v>1.4954709139282634</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>0.54693143168641889</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A82)</f>
+        <v>2.3751354000689271</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>0.76123607523522163</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A83)</f>
+        <v>4.2968399330998359</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>0.45069833677117455</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A84)</f>
+        <v>1.7973225321961135</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>0.57469175675568895</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A85)</f>
+        <v>2.5648232841688747</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>0.56864190888627564</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A86)</f>
+        <v>2.5224500879467007</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>0.92376716786498192</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A87)</f>
+        <v>7.7218891235185154</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>0.80922055662557812</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A88)</f>
+        <v>4.9699117946999873</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>0.74822701327122476</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A89)</f>
+        <v>4.1376823313729689</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>0.97772429420837514</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A90)</f>
+        <v>11.412775862270612</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>0.38804907369484332</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A91)</f>
+        <v>1.4733095563822498</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>0.81690355843927831</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A92)</f>
+        <v>5.0932267856820257</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>0.23781090068026633</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A93)</f>
+        <v>0.81468177673687592</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>0.72144630776841023</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A94)</f>
+        <v>3.8344333422565531</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>1.1142469896511242E-3</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A95)</f>
+        <v>3.3446046730306895E-3</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>7.8631740363009461E-2</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A96)</f>
+        <v>0.24568642514223421</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>9.5274252332576248E-2</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A97)</f>
+        <v>0.30037026737986516</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>4.1135510269063702E-2</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A98)</f>
+        <v>0.12601655341398504</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>6.1715924717818504E-2</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A99)</f>
+        <v>0.19110757113947005</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>0.21797932485098637</v>
+        <f>-3*LN(1-'random-100-numbers-original'!A100)</f>
+        <v>0.73762229993053441</v>
       </c>
     </row>
   </sheetData>
@@ -901,617 +1519,2232 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BD8CAE-D53D-4F1C-B0AF-70A90225B578}">
-  <dimension ref="A1:A100"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216C028-A002-4466-A109-9CC73D8B53F3}">
+  <dimension ref="A1:A200"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection sqref="A1:A100"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A1)</f>
-        <v>1.9471999251808469</v>
+        <v>0.51850546213660853</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A2)</f>
-        <v>1.5940345233077402</v>
+        <v>0.83863176710143517</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A3)</f>
-        <v>1.0689352634953835</v>
+        <v>0.439465239857454</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A4)</f>
-        <v>2.4698655389211561</v>
+        <v>0.94662429294873529</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A5)</f>
-        <v>2.4182816995170215</v>
+        <v>0.71078445387425626</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A6)</f>
-        <v>0.38942996113342676</v>
+        <v>0.28922835794200796</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A7)</f>
-        <v>0.80724206134937759</v>
+        <v>0.69120557869291044</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A8)</f>
-        <v>0.88712758524196822</v>
+        <v>0.71000493881719073</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A9)</f>
-        <v>0.72857762006225502</v>
+        <v>1.7072165926949712E-2</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A10)</f>
-        <v>4.5111434054786272</v>
+        <v>0.70422750109473131</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A11)</f>
-        <v>0.22482099062346594</v>
+        <v>0.83540521690310565</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A12)</f>
-        <v>1.3229111822885704</v>
+        <v>0.13416294265335982</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A13)</f>
-        <v>9.4449337333764554</v>
+        <v>0.35314381596421229</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A14)</f>
-        <v>0.51695461523857833</v>
+        <v>0.57232755861244555</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A15)</f>
-        <v>8.0000442541683778</v>
+        <v>0.15439980258105057</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A16)</f>
-        <v>3.6726571740739802</v>
+        <v>0.28824318339103483</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A17)</f>
-        <v>5.4200607799973746</v>
+        <v>0.94155886948818335</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A18)</f>
-        <v>1.2401544674217029</v>
+        <v>0.21367779109038776</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A19)</f>
-        <v>3.4638948964138319</v>
+        <v>0.69460097215004279</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A20)</f>
-        <v>2.6806949746698949</v>
+        <v>0.2806036453546823</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A21)</f>
-        <v>0.41990700192564312</v>
+        <v>0.21649445882134044</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A22)</f>
-        <v>6.3265446359887108</v>
+        <v>0.64156569765779825</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A23)</f>
-        <v>0.70832564572745715</v>
+        <v>0.51779944563569158</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A24)</f>
-        <v>3.3374555033828415</v>
+        <v>0.78493541158048408</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A25)</f>
-        <v>4.8519429465519135</v>
+        <v>0.28896284633944813</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A26)</f>
-        <v>1.0148402786742743</v>
+        <v>0.56063811318857659</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A27)</f>
-        <v>1.4356501074687413</v>
+        <v>0.86035231437489812</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A28)</f>
-        <v>1.4569484177885792</v>
+        <v>0.37366374967006144</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A29)</f>
-        <v>3.8737644337298951</v>
+        <v>0.81759189397595766</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A30)</f>
-        <v>0.17557902542196074</v>
+        <v>0.8969690227613083</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A31)</f>
-        <v>4.1443705583694399</v>
+        <v>0.83354059949633708</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A32)</f>
-        <v>2.175626942531645</v>
+        <v>0.50647549011129755</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A33)</f>
-        <v>3.6368686978475164</v>
+        <v>0.68624182107960374</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A34)</f>
-        <v>1.0616640070516028</v>
+        <v>0.47864005979912716</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A35)</f>
-        <v>4.8611669990977422</v>
+        <v>0.12908274688113563</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A36)</f>
-        <v>0.95897663222541341</v>
+        <v>0.38603613554188676</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A37)</f>
-        <v>2.0917839648474823</v>
+        <v>0.97228699902403037</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A38)</f>
-        <v>3.0760473775440862</v>
+        <v>0.44546854757959153</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A39)</f>
-        <v>1.8308522777673499</v>
+        <v>0.64156736319928742</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A40)</f>
-        <v>7.5698703171821169</v>
+        <v>0.2241795444160174</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A41)</f>
-        <v>2.0828456308061374</v>
+        <v>6.287007639188269E-2</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A42)</f>
-        <v>1.9188858552023573</v>
+        <v>9.4651829391020237E-2</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A43)</f>
-        <v>0.565645057195998</v>
+        <v>0.52795696993677588</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A44)</f>
-        <v>0.40689148151794485</v>
+        <v>0.54405884119579795</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A45)</f>
-        <v>2.1809481234459041</v>
+        <v>0.4439024332781355</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A46)</f>
-        <v>6.302602789946631</v>
+        <v>0.3200763713097895</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A47)</f>
-        <v>2.6954529436841868</v>
+        <v>0.90171512353692895</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A48)</f>
-        <v>0.97576865365010579</v>
+        <v>0.20996488773271793</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A49)</f>
-        <v>2.4062328125937267</v>
+        <v>0.65895708858146096</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A50)</f>
-        <v>6.4741159808622335</v>
+        <v>0.68063268996030513</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A51)</f>
-        <v>3.4231052944034852</v>
+        <v>0.25979981397401974</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A52)</f>
-        <v>0.64834283734814957</v>
+        <v>0.22297256728539927</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A53)</f>
-        <v>0.3206834065030425</v>
+        <v>0.76683830984313528</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A54)</f>
-        <v>3.67411233863348</v>
+        <v>0.71751813188263724</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A55)</f>
-        <v>14.338481346257151</v>
+        <v>0.88438945984340478</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A56)</f>
-        <v>3.337679984745602</v>
+        <v>0.26677418867147917</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A57)</f>
-        <v>2.3204605324025724</v>
+        <v>0.43242831500119994</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A58)</f>
-        <v>0.58263315668412718</v>
+        <v>4.979262923368255E-2</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A59)</f>
-        <v>5.5344973247597249</v>
+        <v>0.20043473050609895</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A60)</f>
-        <v>6.9936784439094526E-2</v>
+        <v>0.16417970640239188</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A61)</f>
-        <v>3.4125606244095321</v>
+        <v>0.69358119054450362</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A62)</f>
-        <v>3.7532936690291629</v>
+        <v>0.93908986841738729</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A63)</f>
-        <v>10.784365020930196</v>
+        <v>0.5686732927600725</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A64)</f>
-        <v>1.6747417122290291</v>
+        <v>0.31116819793431927</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A65)</f>
-        <v>3.0709641537970516</v>
+        <v>0.93373195852321378</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A66)</f>
-        <v>3.7617827936409185</v>
+        <v>0.74513243752476799</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A67)</f>
-        <v>1.9543534107760285</v>
+        <v>2.8743286699170811E-2</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A68)</f>
-        <v>5.5669362120917025</v>
+        <v>0.9341223488198882</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A69)</f>
-        <v>5.1728931710476038</v>
+        <v>0.6672239679934473</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A70)</f>
-        <v>0.6180320992658328</v>
+        <v>0.37142456035059646</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A71)</f>
-        <v>4.547536523824169</v>
+        <v>9.0146839956378733E-3</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A72)</f>
-        <v>5.4942565628695617</v>
+        <v>0.84861105428924311</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A73)</f>
-        <v>1.517127609945653</v>
+        <v>0.59804255408342233</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A74)</f>
-        <v>0.31906890858941545</v>
+        <v>0.68677101900675086</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A75)</f>
-        <v>5.8886360734214271</v>
+        <v>0.72045701234424808</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A76)</f>
-        <v>0.18453081171161098</v>
+        <v>0.55459927478672288</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A77)</f>
-        <v>2.9679512383118034</v>
+        <v>0.86957338376404048</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A78)</f>
-        <v>0.66538917201115411</v>
+        <v>0.25020933863458372</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A79)</f>
-        <v>2.6944128639485134</v>
+        <v>0.24765645560125771</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A80)</f>
-        <v>2.190493965114094</v>
+        <v>0.90102594724103391</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A81)</f>
-        <v>1.4954709139282634</v>
+        <v>0.62875795980389326</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A82)</f>
-        <v>2.3751354000689271</v>
+        <v>0.79749489321668288</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A83)</f>
-        <v>4.2968399330998359</v>
+        <v>0.57762439654587716</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A84)</f>
-        <v>1.7973225321961135</v>
+        <v>0.67231081204705667</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A85)</f>
-        <v>2.5648232841688747</v>
+        <v>0.17528473746936868</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A86)</f>
-        <v>2.5224500879467007</v>
+        <v>0.2854733867370568</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A87)</f>
-        <v>7.7218891235185154</v>
+        <v>0.72721162537006157</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A88)</f>
-        <v>4.9699117946999873</v>
+        <v>0.71260023475412826</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A89)</f>
-        <v>4.1376823313729689</v>
+        <v>0.67315158118359886</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A90)</f>
-        <v>11.412775862270612</v>
+        <v>0.97284424164968597</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A91)</f>
-        <v>1.4733095563822498</v>
+        <v>0.71587372220454104</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A92)</f>
-        <v>5.0932267856820257</v>
+        <v>0.14872284144830505</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A93)</f>
-        <v>0.81468177673687592</v>
+        <v>6.9520420985936804E-2</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A94)</f>
-        <v>3.8344333422565531</v>
+        <v>0.27429126225607348</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A95)</f>
-        <v>3.3446046730306895E-3</v>
+        <v>0.71352363840357558</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A96)</f>
-        <v>0.24568642514223421</v>
+        <v>0.18221764248045791</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A97)</f>
-        <v>0.30037026737986516</v>
+        <v>6.1095919957847244E-2</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A98)</f>
-        <v>0.12601655341398504</v>
+        <v>0.20463376382091703</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A99)</f>
-        <v>0.19110757113947005</v>
+        <v>0.28190584952734299</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <f>-3*LN(1-'random-numbers-original'!A100)</f>
-        <v>0.73762229993053441</v>
+        <v>0.39572776896214323</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>0.48322510275898267</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>0.31652749872143782</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>0.4160715334707058</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>0.95078860898295592</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>0.38590463326998536</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>0.43950332464961206</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>1.4020115292851409E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>0.20467502330132481</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>3.6526056252219274E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>5.7407025533273814E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>3.0683254620638367E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>0.56310285053337394</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>0.21158309663714547</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>6.0779975658684204E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>0.98297970853509531</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>0.43577189772954905</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>0.63426189267464106</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>0.40435724518379412</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>2.8243226076706041E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>0.82831137504612318</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>0.72395055552367316</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>0.7039288648841342</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>0.20920501009744719</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>0.86773485057579158</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>0.23878388622627611</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>0.11374001890081087</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>0.55476059965516777</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>0.76027398039334204</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>0.35354941974800969</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>0.15952039019148734</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>0.7402873957997339</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>0.87299764432977156</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>0.33089959145785874</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>0.21229988168223257</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>0.44029093068260461</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>0.25940854485206699</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>0.3250192730823187</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>0.34450319919049699</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>0.42283443138752452</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>0.37581752111380207</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>0.67958804512537763</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>0.78933468098879289</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>0.75399307460831955</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>0.23081356993616575</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>0.53246939878365107</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>0.65246836758740179</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>0.16641198987012196</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>0.34341169928692439</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>0.87385274786541178</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>0.17050749666578524</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>0.89674891739924611</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>0.50730326080785093</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>0.88965900908785467</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>0.46903776388652463</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>9.9209017519297227E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>0.86620634205204661</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>0.28342937129221024</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>0.66600250701005792</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>0.32894627109590802</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>0.42641898167699488</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>0.91484679479316078</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>0.32544641178518086</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>0.65131797048728945</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>0.47685473307551662</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>0.37004794322698153</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>0.37964340254889073</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>0.46198099353197231</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>0.43298497058860985</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>0.5102028961457189</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>0.66682473890461402</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>0.62620175386360111</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>8.4758146915420163E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>0.67086925174055356</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>1.7161496068549775E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>0.58379577544283567</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>0.11049455400014752</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>0.37756692148577786</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>0.74555244499937801</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>0.44327159670086291</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>0.97016011037121486</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>0.21358821539872008</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>0.73340351266458104</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>0.91278045174871192</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>0.53856680310632821</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>0.28783397232809715</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>0.75146041925082041</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>0.40275896791563293</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>0.2687374036602499</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>0.86025326378161604</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>0.50740938353210008</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>0.10502273798349737</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>0.89142181204881343</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>0.58535389031613216</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>0.18491333359428452</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>0.89858033488039135</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>0.83199422707909809</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>0.98251389253083299</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>0.77830325264983724</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>0.3333428973483441</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>0.9946343301537609</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BCDC02-4CDA-4240-BADE-2264D816EEC6}">
+  <dimension ref="A1:A200"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="D197" sqref="D197"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A1)</f>
+        <v>2.192581175428693</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A2)</f>
+        <v>5.4721990941243801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A3)</f>
+        <v>1.7365920662443295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A4)</f>
+        <v>8.7911986819769545</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A5)</f>
+        <v>3.7217491035623653</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A6)</f>
+        <v>1.0242122379235967</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A7)</f>
+        <v>3.5252385801302593</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A8)</f>
+        <v>3.7136741596522271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A9)</f>
+        <v>5.165872648275309E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A10)</f>
+        <v>3.6544941148508503</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A11)</f>
+        <v>5.4128060570130216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A12)</f>
+        <v>0.43217563083610422</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A13)</f>
+        <v>1.3068938712970801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A14)</f>
+        <v>2.5481931008130245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A15)</f>
+        <v>0.50312583288005519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A16)</f>
+        <v>1.0200569268541697</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A17)</f>
+        <v>8.5192060423727334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A18)</f>
+        <v>0.72116590666146019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A19)</f>
+        <v>3.5584082082155071</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A20)</f>
+        <v>0.98802844484623664</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A21)</f>
+        <v>0.73193143461217902</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A22)</f>
+        <v>3.0780296784032339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A23)</f>
+        <v>2.1881854907380291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A24)</f>
+        <v>4.6104506541460122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A25)</f>
+        <v>1.0230917851322829</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A26)</f>
+        <v>2.4672955858724777</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A27)</f>
+        <v>5.9058976782277632</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A28)</f>
+        <v>1.4036037329656323</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A29)</f>
+        <v>5.1045262842242689</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A30)</f>
+        <v>6.8181767582354196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A31)</f>
+        <v>5.3790115203434574</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A32)</f>
+        <v>2.1185482677417564</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A33)</f>
+        <v>3.4773981618112071</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A34)</f>
+        <v>1.9539438349690794</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A35)</f>
+        <v>0.41462492640710302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A36)</f>
+        <v>1.4634576157228916</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A37)</f>
+        <v>10.757560879757394</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A38)</f>
+        <v>1.7688952550147237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A39)</f>
+        <v>3.0780436185759337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A40)</f>
+        <v>0.76150247171879415</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A41)</f>
+        <v>0.19480004166742287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A42)</f>
+        <v>0.29830707108781118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A43)</f>
+        <v>2.2520553964911194</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A44)</f>
+        <v>2.3561745465117472</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A45)</f>
+        <v>1.7604345612322061</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A46)</f>
+        <v>1.1573243936069988</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A47)</f>
+        <v>6.9596553434961841</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A48)</f>
+        <v>0.70703366580242399</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A49)</f>
+        <v>3.2272409090362091</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A50)</f>
+        <v>3.4242401894029459</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A51)</f>
+        <v>0.90250382313473154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A52)</f>
+        <v>0.75683886989619764</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A53)</f>
+        <v>4.3680693507501998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A54)</f>
+        <v>3.7924227423325605</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A55)</f>
+        <v>6.4725844472252607</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A56)</f>
+        <v>0.93090467990817061</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A57)</f>
+        <v>1.6991646612762601</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A58)</f>
+        <v>0.15322509957324668</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A59)</f>
+        <v>0.67106133644778354</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A60)</f>
+        <v>0.53802494644824217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A61)</f>
+        <v>3.5484073633127298</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A62)</f>
+        <v>8.3950672615703041</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A63)</f>
+        <v>2.5226683637795695</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A64)</f>
+        <v>1.1182744700642595</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A65)</f>
+        <v>8.1421425810341965</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A66)</f>
+        <v>4.1010336947446042</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A67)</f>
+        <v>8.749339590816603E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A68)</f>
+        <v>8.1598680819361462</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A69)</f>
+        <v>3.300856775519013</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A70)</f>
+        <v>1.3928976806731297</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A71)</f>
+        <v>2.7166686341193638E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A72)</f>
+        <v>5.6637088633317534</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A73)</f>
+        <v>2.7342271556854847</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A74)</f>
+        <v>3.4824623617181283</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A75)</f>
+        <v>3.8237975886747524</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A76)</f>
+        <v>2.4263426877930439</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A77)</f>
+        <v>6.1108336142360997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A78)</f>
+        <v>0.86388368877586452</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A79)</f>
+        <v>0.85368665518974529</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A80)</f>
+        <v>6.9386926696313616</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A81)</f>
+        <v>2.9727030889328607</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A82)</f>
+        <v>4.7909705222114436</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A83)</f>
+        <v>2.5855809156966738</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A84)</f>
+        <v>3.34706915267091</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A85)</f>
+        <v>0.57815126564163943</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A86)</f>
+        <v>1.0084051047359388</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A87)</f>
+        <v>3.8971769067413065</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A88)</f>
+        <v>3.7406433664732672</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A89)</f>
+        <v>3.3547762997341559</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A90)</f>
+        <v>10.818498483470139</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A91)</f>
+        <v>3.7750094985576093</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A92)</f>
+        <v>0.48305255312452544</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A93)</f>
+        <v>0.21616544817296751</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A94)</f>
+        <v>0.96181959700557262</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A95)</f>
+        <v>3.7502977612443553</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A96)</f>
+        <v>0.60347713315024443</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A97)</f>
+        <v>0.18912586851443181</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A98)</f>
+        <v>0.68685778789979857</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A99)</f>
+        <v>0.99346376921562007</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A100)</f>
+        <v>1.5111914068481074</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A101)</f>
+        <v>1.9804437034305513</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A102)</f>
+        <v>1.1417065675383191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A103)</f>
+        <v>1.6139303774279394</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A104)</f>
+        <v>9.0348904726347659</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A105)</f>
+        <v>1.4628151274663108</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A106)</f>
+        <v>1.7367959041973084</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A107)</f>
+        <v>4.2357976479395251E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A108)</f>
+        <v>0.68701341639670477</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A109)</f>
+        <v>0.11162950448190118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A110)</f>
+        <v>0.17736215362855678</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A111)</f>
+        <v>9.3491525664222197E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A112)</f>
+        <v>2.48417240249612</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A113)</f>
+        <v>0.71318479154582848</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A114)</f>
+        <v>0.18811652849880894</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A115)</f>
+        <v>12.22004709340807</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A116)</f>
+        <v>1.7168900177903996</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A117)</f>
+        <v>3.0175132664022009</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A118)</f>
+        <v>1.5543425889071418</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A119)</f>
+        <v>8.5949215272899809E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A120)</f>
+        <v>5.2862182884417521</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A121)</f>
+        <v>3.861525847969423</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A122)</f>
+        <v>3.6514665965797173</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A123)</f>
+        <v>0.70414956955671426</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A124)</f>
+        <v>6.0688399901773682</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A125)</f>
+        <v>0.8185139246248414</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A126)</f>
+        <v>0.36223481708417754</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A127)</f>
+        <v>2.4274294895140516</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A128)</f>
+        <v>4.2847757781505926</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A129)</f>
+        <v>1.3087755770530318</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A130)</f>
+        <v>0.52134775807495204</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A131)</f>
+        <v>4.0445388833922271</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A132)</f>
+        <v>6.1906489323332776</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A133)</f>
+        <v>1.2054634278269221</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A134)</f>
+        <v>0.71591346619870011</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A135)</f>
+        <v>1.7410144479774439</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A136)</f>
+        <v>0.90091844493493944</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A137)</f>
+        <v>1.17921342369537</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A138)</f>
+        <v>1.2670855689749825</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A139)</f>
+        <v>1.6488783189007119</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A140)</f>
+        <v>1.4139375577522006</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A141)</f>
+        <v>3.4144432564237639</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A142)</f>
+        <v>4.6724537118676537</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A143)</f>
+        <v>4.2071867743420004</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A144)</f>
+        <v>0.7872657211374241</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A145)</f>
+        <v>2.2808714257450515</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A146)</f>
+        <v>3.170698768784018</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A147)</f>
+        <v>0.54604797398395033</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A148)</f>
+        <v>1.2620942761659011</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A149)</f>
+        <v>6.2109161599691571</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A150)</f>
+        <v>0.56082362089274818</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A151)</f>
+        <v>6.8117746858759158</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A152)</f>
+        <v>2.1235842830884675</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A153)</f>
+        <v>6.6125393719318852</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A154)</f>
+        <v>1.8991931360988006</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A155)</f>
+        <v>2.9911325474524013E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A156)</f>
+        <v>6.0343695957105821</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A157)</f>
+        <v>0.99983538588735676</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A158)</f>
+        <v>3.2898653761552334</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A159)</f>
+        <v>1.196718217001145</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A160)</f>
+        <v>1.6675682472861753</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A161)</f>
+        <v>7.3899096920789553</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A162)</f>
+        <v>1.1811124730741185</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A163)</f>
+        <v>3.1607845868883961</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A164)</f>
+        <v>1.9436882893763237</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A165)</f>
+        <v>1.3863346885578784</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A166)</f>
+        <v>1.432382427309862</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A167)</f>
+        <v>1.8595841743106567</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A168)</f>
+        <v>1.7021084061218739</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A169)</f>
+        <v>2.1412921421893585</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A170)</f>
+        <v>3.297259853574773</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A171)</f>
+        <v>2.9521172278669008</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A172)</f>
+        <v>2.5535816021500762E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A173)</f>
+        <v>3.3339005881221375</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A174)</f>
+        <v>5.1931383939342463E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A175)</f>
+        <v>2.6297376443057416</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A176)</f>
+        <v>0.35126894806320752</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A177)</f>
+        <v>1.4223574824513296</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A178)</f>
+        <v>4.105981604854561</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A179)</f>
+        <v>1.7570332927760037</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A180)</f>
+        <v>10.535727607262015</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A181)</f>
+        <v>0.72082417426882117</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A182)</f>
+        <v>3.9660571413313668</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A183)</f>
+        <v>7.3179803879924545</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A184)</f>
+        <v>2.3202539629296561</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A185)</f>
+        <v>1.0183326294632822</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A186)</f>
+        <v>4.1764595023806699</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A187)</f>
+        <v>1.5463035247060262</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A188)</f>
+        <v>0.93894796446201512</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A189)</f>
+        <v>5.9037705649494479</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A190)</f>
+        <v>2.1242305273991242</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A191)</f>
+        <v>0.33287089979448625</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A192)</f>
+        <v>6.6608542177495451</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A193)</f>
+        <v>2.6409896108920483</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A194)</f>
+        <v>0.61338249674029088</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A195)</f>
+        <v>6.8654648116122345</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A196)</f>
+        <v>5.3512708126345299</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A197)</f>
+        <v>12.13904571669077</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A198)</f>
+        <v>4.5193345016086788</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A199)</f>
+        <v>1.2164383627007571</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <f>-3*LN(1-'random-200-numbers-original'!A200)</f>
+        <v>15.683202167546998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>